<commit_message>
+Added Mappers for primitives and strings. +Fixed Object Mapper
</commit_message>
<xml_diff>
--- a/lineChart.xlsx
+++ b/lineChart.xlsx
@@ -89,7 +89,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>563266.0</c:v>
+                  <c:v>587224.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -124,7 +124,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6754777.0</c:v>
+                  <c:v>6666786.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -159,7 +159,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>968139.0</c:v>
+                  <c:v>805252.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -194,7 +194,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>766882.0</c:v>
+                  <c:v>609365.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -229,7 +229,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5648430.0</c:v>
+                  <c:v>5202620.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -345,19 +345,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>563266.0</v>
+        <v>587224.0</v>
       </c>
       <c r="B2" t="n">
-        <v>6754777.0</v>
+        <v>6666786.0</v>
       </c>
       <c r="C2" t="n">
-        <v>968139.0</v>
+        <v>805252.0</v>
       </c>
       <c r="D2" t="n">
-        <v>766882.0</v>
+        <v>609365.0</v>
       </c>
       <c r="E2" t="n">
-        <v>5648430.0</v>
+        <v>5202620.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+Added CollectionMapper class and MapMapper class
</commit_message>
<xml_diff>
--- a/lineChart.xlsx
+++ b/lineChart.xlsx
@@ -89,7 +89,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>587224.0</c:v>
+                  <c:v>584146.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -124,7 +124,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6666786.0</c:v>
+                  <c:v>7388145.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -159,7 +159,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>805252.0</c:v>
+                  <c:v>1353054.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -194,7 +194,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>609365.0</c:v>
+                  <c:v>573276.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -229,7 +229,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5202620.0</c:v>
+                  <c:v>5422733.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -345,19 +345,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>587224.0</v>
+        <v>584146.0</v>
       </c>
       <c r="B2" t="n">
-        <v>6666786.0</v>
+        <v>7388145.0</v>
       </c>
       <c r="C2" t="n">
-        <v>805252.0</v>
+        <v>1353054.0</v>
       </c>
       <c r="D2" t="n">
-        <v>609365.0</v>
+        <v>573276.0</v>
       </c>
       <c r="E2" t="n">
-        <v>5202620.0</v>
+        <v>5422733.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>